<commit_message>
Removing charaters that rendered badly on html. Adding Lydia's paper
</commit_message>
<xml_diff>
--- a/conference/pagegen/data/aaai-20.xlsx
+++ b/conference/pagegen/data/aaai-20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Authors</t>
   </si>
@@ -66,9 +66,6 @@
     <t>D3BA: A Tool for Optimizing Business Processes Using Non-Deterministic Planning</t>
   </si>
   <si>
-    <t>Tathagata Chakraborti and Yasaman Khazaeni</t>
-  </si>
-  <si>
     <t>https://arxiv.org/abs/2001.02619</t>
   </si>
   <si>
@@ -102,17 +99,35 @@
     <t>AAAI WS on Intelligent Process Automation Talk on Friday February 7th 15:10-15:30</t>
   </si>
   <si>
-    <t>AAAI 2020 Workshop on Interactive and Conversational Recommendation Systems (WICRS). Presentation on Saturday February 8th 11:40–11:52</t>
-  </si>
-  <si>
-    <t>AAAI Paper Talk on February 11th 9:30-10:45 (Gibson, Tech Sess 9: Planning), Poster on February 11 18:30–20:30 PM (American's Hall 1/2)</t>
+    <t>Reddit: A Novel Online Financial Consultancy</t>
+  </si>
+  <si>
+    <t>The AAAI-20 Workshop on Knowledge Discovery from Unstructured Data in Financial Services</t>
+  </si>
+  <si>
+    <t>https://aaai-kdf2020.github.io/assets/pdfs/kdf2020_paper_30.pdf</t>
+  </si>
+  <si>
+    <t>Social media forums are becoming rich and valuabledata sources due to their features and the level of userengagement on these venues. This paper investigatesdata from online social media forums – which are pop-ular finance-related subreddits to provide answers tofive different research questions proposed in this pa-per. Our analysis revealed five main interesting insights.1) We found that users primarily seek information andshare information on these subreddits. 2) We found thatfinance-related subreddits are highly negative in senti-ment contrary to the popular belief that Reddit postsare in general positive in sentiment. 3) Users on thesesubreddits do not focus much on their past nor futurebut their present situation. 4) Even though overall sen-timent is negative across the subreddits we considered,word-wise, positive emotion dominates negative emo-tion. 5) All these four subreddits have large instances ofdifferent set of pronouns which provide insights aboutwhom the users are addressing in their posts. Overall,we found the patterns of seeking personal advice as wellas sharing experiences of financial decision-making aredominating compared to any other interests.</t>
+  </si>
+  <si>
+    <t>Tathagata Chakraborti and Yasaman Khazaeni</t>
+  </si>
+  <si>
+    <t>AAAI 2020 Workshop on Interactive and Conversational Recommendation Systems (WICRS). Presentation on Saturday February 8th 11:40-11:52</t>
+  </si>
+  <si>
+    <t>AAAI Paper Talk on February 11th 9:30-10:45 (Gibson, Tech Sess 9: Planning), Poster on February 11 18:30-20:30 PM (American's Hall 1/2)</t>
+  </si>
+  <si>
+    <t>Lydia Manikonda and Shailesh Divey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +172,14 @@
       <color rgb="FF1D1C1D"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,7 +211,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -198,6 +220,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -538,125 +563,136 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://arxiv.org/abs/1910.08137"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing dates and links
</commit_message>
<xml_diff>
--- a/conference/pagegen/data/aaai-20.xlsx
+++ b/conference/pagegen/data/aaai-20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Authors</t>
   </si>
@@ -93,9 +93,6 @@
     <t>AAAI Debate Monday 6:15-7:15pm; Grand Ballroom</t>
   </si>
   <si>
-    <t>AAAI Tutorial on Feb 7 2-6pm (Gibson, 2nd floor)</t>
-  </si>
-  <si>
     <t>AAAI WS on Intelligent Process Automation Talk on Friday February 7th 15:10-15:30</t>
   </si>
   <si>
@@ -118,6 +115,12 @@
   </si>
   <si>
     <t>Lydia Manikonda and Shailesh Divey</t>
+  </si>
+  <si>
+    <t>https://aaai-kdf2020.github.io/</t>
+  </si>
+  <si>
+    <t>AAAI Tutorial on Feb 8 2-6pm (Gibson, 2nd floor)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -560,10 +563,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
@@ -574,17 +577,19 @@
     </row>
     <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -595,7 +600,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -625,7 +630,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>

</xml_diff>